<commit_message>
Documentación de Dynamo para reducción de costos
</commit_message>
<xml_diff>
--- a/Dynamo/DynamoDB.xlsx
+++ b/Dynamo/DynamoDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\50241\Desktop\Github\FEL_ENERGUATE\FEL_DOCUMENTACION\Dynamo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73908F44-5FB8-43EA-93CE-861C950A1E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A77EB51-8DD2-4E9D-B056-4FE8A538C71E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2610" windowWidth="29040" windowHeight="15840" xr2:uid="{B8AF0390-AA7B-41D9-B0FC-99645A3E555F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8AF0390-AA7B-41D9-B0FC-99645A3E555F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>Indice</t>
   </si>
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,8 +176,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +213,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -290,12 +302,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -305,6 +318,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,10 +331,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -636,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E282AEB3-0B50-4F80-B722-A377AE2C7343}">
   <dimension ref="B1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,42 +682,42 @@
   <sheetData>
     <row r="1" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
     </row>
     <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
@@ -806,7 +825,9 @@
       <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -891,110 +912,110 @@
       <c r="AG6" s="3"/>
     </row>
     <row r="7" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="S7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="T7" s="4" t="s">
+      <c r="T7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="U7" s="4" t="s">
+      <c r="U7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="V7" s="4" t="s">
+      <c r="V7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="W7" s="4" t="s">
+      <c r="W7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="X7" s="4" t="s">
+      <c r="X7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="Y7" s="4" t="s">
+      <c r="Y7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Z7" s="3" t="s">
+      <c r="Z7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AA7" s="4" t="s">
+      <c r="AA7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AB7" s="4" t="s">
+      <c r="AB7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AC7" s="4" t="s">
+      <c r="AC7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AD7" s="3" t="s">
+      <c r="AD7" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AE7" s="3" t="s">
+      <c r="AE7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AF7" s="13" t="s">
+      <c r="AF7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="AG7" s="13" t="s">
+      <c r="AG7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AH7" s="13" t="s">
+      <c r="AH7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AI7" s="13" t="s">
+      <c r="AI7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="13"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
     </row>
     <row r="8" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">

</xml_diff>